<commit_message>
new figs, scripts for analysing PP diag runs
</commit_message>
<xml_diff>
--- a/scripts/Irradiancetest_SalinityMult_Fit-2.xlsx
+++ b/scripts/Irradiancetest_SalinityMult_Fit-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greig\Documents\github\Ecosystem-Model-Data-Framework\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA60DA1-80EF-4CDF-9457-93CF6DECEDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BE1704-DBE7-47D4-9F9D-F91EBEB93042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{C38FC2C9-5C90-46CF-89CA-BC452CCF3AA7}"/>
   </bookViews>
@@ -34,7 +34,6 @@
     <definedName name="x">'Old - JB experiments'!$Y$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>Mixing Layer thickness</t>
   </si>
@@ -269,6 +268,15 @@
   </si>
   <si>
     <t>Zp = depth of photic zone</t>
+  </si>
+  <si>
+    <t>I_0 / zK *(1-e^(-Kz)</t>
+  </si>
+  <si>
+    <t>Is this sum across depths?</t>
+  </si>
+  <si>
+    <t>crosscheck</t>
   </si>
 </sst>
 </file>
@@ -9419,8 +9427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE4E476-7789-41A8-A99A-C7B8C3DE4629}">
   <dimension ref="B3:BL262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="Q5" workbookViewId="0">
+      <selection activeCell="AG14" sqref="AG14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10051,6 +10059,12 @@
         <f t="shared" si="1"/>
         <v>1.8946137629748092</v>
       </c>
+      <c r="AB23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>74</v>
+      </c>
       <c r="BB23" s="1">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -10081,6 +10095,13 @@
         <f t="shared" si="1"/>
         <v>1.4035643967660916</v>
       </c>
+      <c r="AB24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE24">
+        <f>SUM(P10:P39)</f>
+        <v>361.08637445968083</v>
+      </c>
       <c r="BB24" s="1">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -10110,6 +10131,10 @@
       <c r="P25">
         <f t="shared" si="1"/>
         <v>1.0397860790244648</v>
+      </c>
+      <c r="AB25">
+        <f>I0/(29*K)*(1-EXP(-K*29))</f>
+        <v>6.896548245878189</v>
       </c>
       <c r="AO25" t="s">
         <v>55</v>

</xml_diff>